<commit_message>
vae and pssl other info fixes
</commit_message>
<xml_diff>
--- a/Frontend/src/assets/template File/PSSL - Other Info.xlsx
+++ b/Frontend/src/assets/template File/PSSL - Other Info.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
     <sheet name="Exchange Rates" sheetId="2" r:id="rId2"/>
     <sheet name="Obligor Tiers" sheetId="3" r:id="rId3"/>
+    <sheet name="Obligor Tiers Ebitda" sheetId="4" r:id="rId4"/>
+    <sheet name="Obligor Outstandings" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" calcMode="autoNoTable" iterate="1"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Input</t>
   </si>
@@ -131,14 +133,146 @@
   </si>
   <si>
     <t>85</t>
+  </si>
+  <si>
+    <t>EBITDA</t>
+  </si>
+  <si>
+    <t>Absolute Value</t>
+  </si>
+  <si>
+    <t>Debt-to-Cash Capitalization Ratio</t>
+  </si>
+  <si>
+    <t>Permitted Add-Backs</t>
+  </si>
+  <si>
+    <t>&lt;$10MM</t>
+  </si>
+  <si>
+    <t>&gt;35.0%</t>
+  </si>
+  <si>
+    <r>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>35.0%</t>
+    </r>
+  </si>
+  <si>
+    <t>≥$10MM and &lt; $50MM</t>
+  </si>
+  <si>
+    <t>&gt;50.0%</t>
+  </si>
+  <si>
+    <r>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>50.0%</t>
+    </r>
+  </si>
+  <si>
+    <t>≥$50MM</t>
+  </si>
+  <si>
+    <t>Loan Category</t>
+  </si>
+  <si>
+    <t>Advance Rate (%)</t>
+  </si>
+  <si>
+    <t>First Lien 10mm</t>
+  </si>
+  <si>
+    <t>First Lien 10mm And 50mm</t>
+  </si>
+  <si>
+    <t>First Lien 10mm And 50mm Senior Leverage In Excess Of 6 5x</t>
+  </si>
+  <si>
+    <t>First Lien 10mm And 50mm Senior Leverage In Excess Of 7 5x</t>
+  </si>
+  <si>
+    <t>First Lien 10mm Senior Leverage In Excess Of 6 5x</t>
+  </si>
+  <si>
+    <t>First Lien 10mm Senior Leverage In Excess Of 7 5x</t>
+  </si>
+  <si>
+    <t>First Lien 50mm B Or Better</t>
+  </si>
+  <si>
+    <t>First Lien 50mm B Or Better Senior Leverage In Excess Of 6 5x</t>
+  </si>
+  <si>
+    <t>First Lien 50mm B Or Better Senior Leverage In Excess Of 7 5x</t>
+  </si>
+  <si>
+    <t>First Lien 50mm Unrated</t>
+  </si>
+  <si>
+    <t>First Lien 50mm Unrated Senior Leverage In Excess Of 6 5x</t>
+  </si>
+  <si>
+    <t>First Lien 50mm Unrated Senior Leverage In Excess Of 7 5x</t>
+  </si>
+  <si>
+    <t>Ineligible</t>
+  </si>
+  <si>
+    <t>Last Out</t>
+  </si>
+  <si>
+    <t>Second Lien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="5">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -166,8 +300,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -752,4 +914,235 @@
     <ignoredError sqref="A1:E4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="29.25" customWidth="1"/>
+    <col min="4" max="4" width="24.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="54" customWidth="1"/>
+    <col min="2" max="2" width="24.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="13"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="13"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="13"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="13"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="13"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="13"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="13"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="13"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="13"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="13"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="13"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>